<commit_message>
conexión y consumo con servicios web del login con json y ajax
</commit_message>
<xml_diff>
--- a/Cided_V2_0_Up/Documentación/TiempodeTareas.xlsx
+++ b/Cided_V2_0_Up/Documentación/TiempodeTareas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex-\Documents\NetBeansProjects\crm_investigadores\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex-\Documents\NetBeansProjects\crm_investigadores\Cided_V2_0_Up\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78B8E42-70C6-48DF-B56D-4F586C761DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C40E8-6E27-4B95-93CF-0175234431E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{392DA8E6-D5AF-425E-9FAD-84E6F0D39CCA}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tareas</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Creación de base de datos</t>
+  </si>
+  <si>
+    <t>ServicioWeb Login</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:F193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,12 +510,16 @@
       </c>
       <c r="F3" s="3">
         <f>SUM(B2:B193)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Pantalla principal del Director
</commit_message>
<xml_diff>
--- a/Cided_V2_0_Up/Documentación/TiempodeTareas.xlsx
+++ b/Cided_V2_0_Up/Documentación/TiempodeTareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex-\Documents\NetBeansProjects\crm_investigadores\Cided_V2_0_Up\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C40E8-6E27-4B95-93CF-0175234431E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109EAB6-632E-40E1-B3FC-2247799E0B98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{392DA8E6-D5AF-425E-9FAD-84E6F0D39CCA}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{392DA8E6-D5AF-425E-9FAD-84E6F0D39CCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Tareas</t>
   </si>
@@ -48,13 +49,108 @@
   </si>
   <si>
     <t>ServicioWeb Login</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conexión y consumo del servicioWeb </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con la interfaz</t>
+    </r>
+  </si>
+  <si>
+    <t>UI del Componente de información general para el Director</t>
+  </si>
+  <si>
+    <t>UI del Componente de reloj semaforizado general para el Director</t>
+  </si>
+  <si>
+    <t>UI del menú Director</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,9 +174,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,12 +259,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -473,809 +589,1058 @@
   <dimension ref="A1:F193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="6">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <f>SUM(B2:B193)</f>
-        <v>25</v>
+      <c r="F3" s="7">
+        <f>SUM(C2:C193)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123" s="1"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127" s="1"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" s="1"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182" s="1"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184" s="1"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185" s="1"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C186" s="1"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C187" s="1"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C188" s="1"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C189" s="1"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C190" s="1"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C191" s="1"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C192" s="1"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>